<commit_message>
zarr for future simulations
</commit_message>
<xml_diff>
--- a/scripts/eerie_menus.xlsx
+++ b/scripts/eerie_menus.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,7 +477,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -496,7 +496,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -518,7 +518,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -537,7 +537,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -559,7 +559,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -604,7 +604,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -623,7 +623,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -653,7 +653,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>hist</t>
+          <t>future</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,12 +668,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>decadal/hist_EERIE_clim.zarr</t>
+          <t>decadal/future_EERIE_clim.zarr</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -690,11 +690,11 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>hist</t>
+          <t>future</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -709,12 +709,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>decadal/hist_EERIE_trend.zarr</t>
+          <t>decadal/future_EERIE_trend.zarr</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -731,11 +731,11 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>hist</t>
+          <t>future</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -750,12 +750,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>time_series/hist_EERIE_IPCC_ts.zarr</t>
+          <t>time_series/future_EERIE_IPCC_ts.zarr</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -776,11 +776,11 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>hist</t>
+          <t>future</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -795,12 +795,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>time_series/hist_EERIE_EDDY_ts.zarr</t>
+          <t>time_series/future_EERIE_EDDY_ts.zarr</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>hist-amip</t>
+          <t>hist</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -835,17 +835,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['ifs-amip-tco1279.hist', 'ifs-amip-tco1279.hist-c-0-a-lr20', 'ifs-amip-tco399.hist-c-0-a-lr20', 'ifs-amip-tco399.hist-c-lr20-a-0', 'ifs-amip-tco399.hist']</t>
+          <t>['ifs-fesom', 'icon']</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'tasmax', 'tasmin']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>decadal/hist-amip_EERIE_clim.zarr</t>
+          <t>decadal/hist_EERIE_clim.zarr</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -862,11 +862,11 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>hist-amip</t>
+          <t>hist</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -876,17 +876,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['ifs-amip-tco1279.hist', 'ifs-amip-tco1279.hist-c-0-a-lr20', 'ifs-amip-tco399.hist-c-0-a-lr20', 'ifs-amip-tco399.hist-c-lr20-a-0', 'ifs-amip-tco399.hist']</t>
+          <t>['ifs-fesom', 'icon']</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'tasmax', 'tasmin']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>decadal/hist-amip_EERIE_trend.zarr</t>
+          <t>decadal/hist_EERIE_trend.zarr</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -903,11 +903,11 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>hist-amip</t>
+          <t>hist</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -917,17 +917,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['ifs-amip-tco1279-hist', 'ifs-amip-tco1279-hist-c-0-a-lr20', 'ifs-amip-tco399-hist-c-0-a-lr20_1', 'ifs-amip-tco399-hist-c-0-a-lr20_10', 'ifs-amip-tco399-hist-c-0-a-lr20_2', 'ifs-amip-tco399-hist-c-0-a-lr20_3', 'ifs-amip-tco399-hist-c-0-a-lr20_4', 'ifs-amip-tco399-hist-c-0-a-lr20_5', 'ifs-amip-tco399-hist-c-0-a-lr20_6', 'ifs-amip-tco399-hist-c-0-a-lr20_7', 'ifs-amip-tco399-hist-c-0-a-lr20_8', 'ifs-amip-tco399-hist-c-0-a-lr20_9', 'ifs-amip-tco399-hist-c-lr20-a-0_1', 'ifs-amip-tco399-hist-c-lr20-a-0_10', 'ifs-amip-tco399-hist-c-lr20-a-0_2', 'ifs-amip-tco399-hist-c-lr20-a-0_3', 'ifs-amip-tco399-hist-c-lr20-a-0_4', 'ifs-amip-tco399-hist-c-lr20-a-0_5', 'ifs-amip-tco399-hist-c-lr20-a-0_6', 'ifs-amip-tco399-hist-c-lr20-a-0_7', 'ifs-amip-tco399-hist-c-lr20-a-0_8', 'ifs-amip-tco399-hist-c-lr20-a-0_9', 'ifs-amip-tco399-hist_1', 'ifs-amip-tco399-hist_10', 'ifs-amip-tco399-hist_2', 'ifs-amip-tco399-hist_3', 'ifs-amip-tco399-hist_4', 'ifs-amip-tco399-hist_5', 'ifs-amip-tco399-hist_6', 'ifs-amip-tco399-hist_7', 'ifs-amip-tco399-hist_8', 'ifs-amip-tco399-hist_9']</t>
+          <t>['ifs-fesom', 'icon']</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'tasmax', 'tasmin']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>time_series/hist-amip_EERIE_IPCC_ts.zarr</t>
+          <t>time_series/hist_EERIE_IPCC_ts.zarr</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -948,11 +948,11 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>hist-amip</t>
+          <t>hist</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -962,17 +962,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['ifs-amip-tco1279-hist', 'ifs-amip-tco1279-hist-c-0-a-lr20', 'ifs-amip-tco399-hist-c-0-a-lr20_1', 'ifs-amip-tco399-hist-c-0-a-lr20_10', 'ifs-amip-tco399-hist-c-0-a-lr20_2', 'ifs-amip-tco399-hist-c-0-a-lr20_3', 'ifs-amip-tco399-hist-c-0-a-lr20_4', 'ifs-amip-tco399-hist-c-0-a-lr20_5', 'ifs-amip-tco399-hist-c-0-a-lr20_6', 'ifs-amip-tco399-hist-c-0-a-lr20_7', 'ifs-amip-tco399-hist-c-0-a-lr20_8', 'ifs-amip-tco399-hist-c-0-a-lr20_9', 'ifs-amip-tco399-hist-c-lr20-a-0_1', 'ifs-amip-tco399-hist-c-lr20-a-0_10', 'ifs-amip-tco399-hist-c-lr20-a-0_2', 'ifs-amip-tco399-hist-c-lr20-a-0_3', 'ifs-amip-tco399-hist-c-lr20-a-0_4', 'ifs-amip-tco399-hist-c-lr20-a-0_5', 'ifs-amip-tco399-hist-c-lr20-a-0_6', 'ifs-amip-tco399-hist-c-lr20-a-0_7', 'ifs-amip-tco399-hist-c-lr20-a-0_8', 'ifs-amip-tco399-hist-c-lr20-a-0_9', 'ifs-amip-tco399-hist_1', 'ifs-amip-tco399-hist_10', 'ifs-amip-tco399-hist_2', 'ifs-amip-tco399-hist_3', 'ifs-amip-tco399-hist_4', 'ifs-amip-tco399-hist_5', 'ifs-amip-tco399-hist_6', 'ifs-amip-tco399-hist_7', 'ifs-amip-tco399-hist_8', 'ifs-amip-tco399-hist_9']</t>
+          <t>['ifs-fesom', 'icon']</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'tasmax', 'tasmin']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>time_series/hist-amip_EERIE_EDDY_ts.zarr</t>
+          <t>time_series/hist_EERIE_EDDY_ts.zarr</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -993,11 +993,11 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>hist-amip</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1007,17 +1007,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-amip-tco1279.hist', 'ifs-amip-tco1279.hist-c-0-a-lr20', 'ifs-amip-tco399.hist-c-0-a-lr20', 'ifs-amip-tco399.hist-c-lr20-a-0', 'ifs-amip-tco399.hist']</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>decadal/obs_clim.zarr</t>
+          <t>decadal/hist-amip_EERIE_clim.zarr</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>hist-amip</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1048,17 +1048,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-amip-tco1279.hist', 'ifs-amip-tco1279.hist-c-0-a-lr20', 'ifs-amip-tco399.hist-c-0-a-lr20', 'ifs-amip-tco399.hist-c-lr20-a-0', 'ifs-amip-tco399.hist']</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>decadal/obs_trend.zarr</t>
+          <t>decadal/hist-amip_EERIE_trend.zarr</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>hist-amip</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1089,17 +1089,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-amip-tco1279-hist', 'ifs-amip-tco1279-hist-c-0-a-lr20', 'ifs-amip-tco399-hist-c-0-a-lr20_1', 'ifs-amip-tco399-hist-c-0-a-lr20_10', 'ifs-amip-tco399-hist-c-0-a-lr20_2', 'ifs-amip-tco399-hist-c-0-a-lr20_3', 'ifs-amip-tco399-hist-c-0-a-lr20_4', 'ifs-amip-tco399-hist-c-0-a-lr20_5', 'ifs-amip-tco399-hist-c-0-a-lr20_6', 'ifs-amip-tco399-hist-c-0-a-lr20_7', 'ifs-amip-tco399-hist-c-0-a-lr20_8', 'ifs-amip-tco399-hist-c-0-a-lr20_9', 'ifs-amip-tco399-hist-c-lr20-a-0_1', 'ifs-amip-tco399-hist-c-lr20-a-0_10', 'ifs-amip-tco399-hist-c-lr20-a-0_2', 'ifs-amip-tco399-hist-c-lr20-a-0_3', 'ifs-amip-tco399-hist-c-lr20-a-0_4', 'ifs-amip-tco399-hist-c-lr20-a-0_5', 'ifs-amip-tco399-hist-c-lr20-a-0_6', 'ifs-amip-tco399-hist-c-lr20-a-0_7', 'ifs-amip-tco399-hist-c-lr20-a-0_8', 'ifs-amip-tco399-hist-c-lr20-a-0_9', 'ifs-amip-tco399-hist_1', 'ifs-amip-tco399-hist_10', 'ifs-amip-tco399-hist_2', 'ifs-amip-tco399-hist_3', 'ifs-amip-tco399-hist_4', 'ifs-amip-tco399-hist_5', 'ifs-amip-tco399-hist_6', 'ifs-amip-tco399-hist_7', 'ifs-amip-tco399-hist_8', 'ifs-amip-tco399-hist_9']</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'tasmax', 'tasmin']</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>time_series/obs_IPCC_ts.zarr</t>
+          <t>time_series/hist-amip_EERIE_IPCC_ts.zarr</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1124,40 +1124,212 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>hist-amip</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ts</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>['ifs-amip-tco1279-hist', 'ifs-amip-tco1279-hist-c-0-a-lr20', 'ifs-amip-tco399-hist-c-0-a-lr20_1', 'ifs-amip-tco399-hist-c-0-a-lr20_10', 'ifs-amip-tco399-hist-c-0-a-lr20_2', 'ifs-amip-tco399-hist-c-0-a-lr20_3', 'ifs-amip-tco399-hist-c-0-a-lr20_4', 'ifs-amip-tco399-hist-c-0-a-lr20_5', 'ifs-amip-tco399-hist-c-0-a-lr20_6', 'ifs-amip-tco399-hist-c-0-a-lr20_7', 'ifs-amip-tco399-hist-c-0-a-lr20_8', 'ifs-amip-tco399-hist-c-0-a-lr20_9', 'ifs-amip-tco399-hist-c-lr20-a-0_1', 'ifs-amip-tco399-hist-c-lr20-a-0_10', 'ifs-amip-tco399-hist-c-lr20-a-0_2', 'ifs-amip-tco399-hist-c-lr20-a-0_3', 'ifs-amip-tco399-hist-c-lr20-a-0_4', 'ifs-amip-tco399-hist-c-lr20-a-0_5', 'ifs-amip-tco399-hist-c-lr20-a-0_6', 'ifs-amip-tco399-hist-c-lr20-a-0_7', 'ifs-amip-tco399-hist-c-lr20-a-0_8', 'ifs-amip-tco399-hist-c-lr20-a-0_9', 'ifs-amip-tco399-hist_1', 'ifs-amip-tco399-hist_10', 'ifs-amip-tco399-hist_2', 'ifs-amip-tco399-hist_3', 'ifs-amip-tco399-hist_4', 'ifs-amip-tco399-hist_5', 'ifs-amip-tco399-hist_6', 'ifs-amip-tco399-hist_7', 'ifs-amip-tco399-hist_8', 'ifs-amip-tco399-hist_9']</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'tasmax', 'tasmin']</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>time_series/hist-amip_EERIE_EDDY_ts.zarr</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>['value (variable)', 'anomaly (variable_anom)']</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>EDDY</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>['region', 'time_filter']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>obs</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>clim</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>['ifs-fesom', 'icon']</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>decadal/obs_clim.zarr</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['value (variable)', 'anomaly (variable_anom)']</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>['period', 'time_filter']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>obs</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>trend</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>['ifs-fesom', 'icon']</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>decadal/obs_trend.zarr</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>['value (variable with hatching over variable_pvalue &gt; 0.05)']</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>['period', 'time_filter']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>obs</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>ts</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>['ifs-fesom', 'icon']</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin', 'eke']</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>['ifs-fesom', 'icon']</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>time_series/obs_IPCC_ts.zarr</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>['value (variable)', 'anomaly (variable_anom)']</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>IPCC</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>['region', 'time_filter']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>obs</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ts</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>['ifs-fesom', 'icon']</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['sfcWind', 'uas', 'vas', 'tas', 'pr', 'tos', 'clt', 'zos', 'tasmax', 'tasmin']</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
         <is>
           <t>time_series/obs_EDDY_ts.zarr</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['value (variable)', 'anomaly (variable_anom)']</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>['value (variable)', 'anomaly (variable_anom)']</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>EDDY</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>['region', 'time_filter']</t>
         </is>

</xml_diff>

<commit_message>
fix short member mapping
</commit_message>
<xml_diff>
--- a/scripts/eerie_menus.xlsx
+++ b/scripts/eerie_menus.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -491,7 +491,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -573,7 +573,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -663,7 +663,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -704,7 +704,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -790,7 +790,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -835,7 +835,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -917,7 +917,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -962,7 +962,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['ifs-fesom', 'icon']</t>
+          <t>['ifs-fesom', 'icon', 'ifs-nemo-er', 'hadgem3-mediumres', 'hadgem3-hires', 'hadgem3-lowres']</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">

</xml_diff>